<commit_message>
backed out Traffic logic
</commit_message>
<xml_diff>
--- a/Test File/Taylor Johnson- Account List.xlsx
+++ b/Test File/Taylor Johnson- Account List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akulkarni/Documents/WebIntel/Test File/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACB4F04-C01C-9140-A035-D139A6E11541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C09A8F-ADB9-644A-B3B4-A8A889409F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2960" windowWidth="28040" windowHeight="17440" xr2:uid="{70A81594-C6B9-A44B-A863-4DA9C8438A49}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Company</t>
   </si>
@@ -59,13 +59,19 @@
   </si>
   <si>
     <t xml:space="preserve">Outlook, Microsoft Office 365, Google Cloud Hosting, DNS Made Easy, Drupal, SuccessFactors (SAP), WP Engine, New Relic, Bootstrap Framework, Mobile Friendly, Google Tag Manager, Hotjar, Typekit, Cedexis Radar, WordPress.org, Adobe Media Optimizer, Vimeo, </t>
+  </si>
+  <si>
+    <t>http://cloudflare.com</t>
+  </si>
+  <si>
+    <t>http://apple.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -196,6 +202,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -498,7 +512,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -541,11 +555,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -579,6 +595,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -919,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9B471C-53CF-A441-B48D-E6E0F86F58EA}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -972,7 +989,21 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{005AF74E-96EF-094A-A0C3-F4CB3C9A78F7}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{419571C6-CD54-BD4C-845C-B6E6F88FF3D9}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>